<commit_message>
adding demographics, adding commenting and fixing things in the correct choice bias calculation
</commit_message>
<xml_diff>
--- a/demographics for data analysis 6.4.22.xlsx
+++ b/demographics for data analysis 6.4.22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK online replication/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91097711-982C-5A4A-B8E1-6E6714A45DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC1E9AE-6955-C041-8459-B751E9C8FC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="500" windowWidth="15200" windowHeight="16080" xr2:uid="{538D7409-5AD6-C94B-AB06-90D24E29A232}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="15200" windowHeight="16080" activeTab="1" xr2:uid="{538D7409-5AD6-C94B-AB06-90D24E29A232}"/>
   </bookViews>
   <sheets>
     <sheet name="all participants" sheetId="1" r:id="rId1"/>
@@ -978,7 +978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1002,24 +1002,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1349,7 +1342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188AD4CC-E48A-FA4A-AA58-C0E53E3EECE9}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3295,7 +3288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6980A5AF-9905-F445-950E-D7EBA12A665B}">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N6" sqref="N6:U7"/>
     </sheetView>
   </sheetViews>
@@ -3328,7 +3321,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="16" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4040,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB040F8-0F97-CD4B-85FA-A875119D0A9F}">
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4078,7 +4071,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="16" t="s">
         <v>259</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -4201,7 +4194,7 @@
         <f t="shared" ref="AI2:AI41" si="3">DATEDIF(AF2,DATE(2022,4,24),"Y")</f>
         <v>19</v>
       </c>
-      <c r="AK2" s="18" t="s">
+      <c r="AK2" s="6" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4242,13 +4235,13 @@
       <c r="M3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="O3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="17" t="s">
+      <c r="O3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="Q3" s="2">
@@ -4746,7 +4739,7 @@
       <c r="O7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="14" t="s">
         <v>206</v>
       </c>
       <c r="Q7" s="2">
@@ -5546,13 +5539,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="S18" s="20" t="s">
+      <c r="S18" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
       <c r="AE18" s="4" t="s">
         <v>119</v>
       </c>
@@ -5587,19 +5580,19 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="S19" s="21" t="s">
+      <c r="S19" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="T19" s="22">
+      <c r="T19" s="19">
         <v>42603</v>
       </c>
-      <c r="U19" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="V19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="W19" s="21">
+      <c r="U19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="W19" s="18">
         <f t="shared" ref="W19:W26" si="4">DATEDIF(T19,DATE(2022,4,24),"Y")</f>
         <v>5</v>
       </c>
@@ -5637,19 +5630,19 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S20" s="21" t="s">
+      <c r="S20" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="T20" s="23" t="s">
+      <c r="T20" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="U20" s="21" t="s">
+      <c r="U20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V20" s="21" t="s">
+      <c r="V20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="W20" s="21">
+      <c r="W20" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5687,19 +5680,19 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="S21" s="21" t="s">
+      <c r="S21" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="T21" s="23" t="s">
+      <c r="T21" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="U21" s="21" t="s">
+      <c r="U21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="W21" s="21">
+      <c r="V21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="W21" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5737,17 +5730,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S22" s="21" t="s">
+      <c r="S22" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="T22" s="22">
+      <c r="T22" s="19">
         <v>42547</v>
       </c>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21" t="s">
+      <c r="U22" s="18"/>
+      <c r="V22" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="W22" s="21">
+      <c r="W22" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5788,19 +5781,19 @@
       <c r="F23" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="S23" s="21" t="s">
+      <c r="S23" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="T23" s="22">
+      <c r="T23" s="19">
         <v>42653</v>
       </c>
-      <c r="U23" s="21" t="s">
+      <c r="U23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V23" s="21" t="s">
+      <c r="V23" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="W23" s="21">
+      <c r="W23" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5838,19 +5831,19 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="S24" s="21" t="s">
+      <c r="S24" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="T24" s="23" t="s">
+      <c r="T24" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="U24" s="21" t="s">
+      <c r="U24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V24" s="21" t="s">
+      <c r="V24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="W24" s="21">
+      <c r="W24" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5891,19 +5884,19 @@
       <c r="F25" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="S25" s="21" t="s">
+      <c r="S25" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="T25" s="23" t="s">
+      <c r="T25" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="U25" s="21" t="s">
+      <c r="U25" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="21" t="s">
+      <c r="V25" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="W25" s="21">
+      <c r="W25" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5916,7 +5909,7 @@
       <c r="AG25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AH25" s="14" t="s">
+      <c r="AH25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AI25" s="2">
@@ -5941,19 +5934,19 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="S26" s="21" t="s">
+      <c r="S26" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="T26" s="22">
+      <c r="T26" s="19">
         <v>42795</v>
       </c>
-      <c r="U26" s="21" t="s">
+      <c r="U26" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V26" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="W26" s="21">
+      <c r="V26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="W26" s="18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -5966,7 +5959,7 @@
       <c r="AG26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AH26" s="14" t="s">
+      <c r="AH26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AI26" s="2">
@@ -6003,7 +5996,7 @@
       <c r="AG27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AH27" s="15" t="s">
+      <c r="AH27" s="14" t="s">
         <v>206</v>
       </c>
       <c r="AI27" s="2">
@@ -6040,7 +6033,7 @@
       <c r="AG28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AH28" s="14" t="s">
+      <c r="AH28" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AI28" s="2">
@@ -6265,7 +6258,7 @@
       <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="2">
@@ -6299,7 +6292,7 @@
       <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E36" s="2">
@@ -6333,7 +6326,7 @@
       <c r="C37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E37" s="2">
@@ -6367,7 +6360,7 @@
       <c r="C38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E38" s="2">
@@ -6585,7 +6578,7 @@
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="4" t="s">
         <v>255</v>
       </c>
     </row>
@@ -7215,7 +7208,7 @@
       <c r="O6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="14" t="s">
         <v>206</v>
       </c>
       <c r="Q6" s="2">
@@ -7325,7 +7318,7 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E8" s="2">
@@ -7439,7 +7432,7 @@
         <v>42547</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="14" t="s">
         <v>206</v>
       </c>
       <c r="K10" s="2">
@@ -7457,7 +7450,7 @@
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E11" s="2">
@@ -7525,7 +7518,7 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E13" s="2">

</xml_diff>